<commit_message>
Update: Work on White NavBar
</commit_message>
<xml_diff>
--- a/Opciones de menu.xlsx
+++ b/Opciones de menu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\TecNM\Migracion de portal Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YogurtSnek\Documents\Programming\HTML\TECNM_Main_Page\tecnm-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B138C16-867A-45D2-845D-3CD47C19F668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8C89D5-B115-4C2D-8941-246850CE1880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{55D38FD7-4481-4AD3-8345-C4433DDD2258}"/>
+    <workbookView xWindow="11508" yWindow="192" windowWidth="11436" windowHeight="11952" xr2:uid="{55D38FD7-4481-4AD3-8345-C4433DDD2258}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -334,12 +334,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -354,8 +366,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7B15F4-E167-430D-A4EC-E3123BA0787A}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,52 +711,52 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>